<commit_message>
Added Project Json test case Added .variation folder test case Updated Nuspec Removed .variation folder Updated Config + Config_Expected
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/Config_Expected.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/Config_Expected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\Unit_Module_Testing\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergiu Wittenberger\PycharmProjects\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Tests\Cache\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7638925C-5898-4667-940C-C81828151B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC629DD9-F40E-425E-AB7B-AB205D4D7533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="218">
   <si>
     <t>Name</t>
   </si>
@@ -679,6 +679,15 @@
   </si>
   <si>
     <t>Path to the Orchestrator Folder where the Queue resides. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>ClassificationThreshold</t>
+  </si>
+  <si>
+    <t>Classification threshold for Classification Business Rule Validation must be a value between 0 and 1.</t>
+  </si>
+  <si>
+    <t>DU_ClassificationThreshold</t>
   </si>
 </sst>
 </file>
@@ -1077,10 +1086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1311,64 +1320,78 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="3"/>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" t="s">
-        <v>210</v>
-      </c>
-    </row>
+        <v>215</v>
+      </c>
+      <c r="B22">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B24" s="3"/>
       <c r="C24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="3"/>
+        <v>37</v>
+      </c>
       <c r="C26" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>79</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="3"/>
+    </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2341,6 +2364,8 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" xr:uid="{EF98B574-7169-43E5-821B-D4670F472688}"/>
@@ -3793,8 +3818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3968,7 +3993,17 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4966,7 +5001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated python tests as well
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/Config_Expected.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/Config_Expected.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath Projects\UiPath Internal Projects\DU Process\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Tests\Cache\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath Projects\UiPath Internal Projects\DU Process\StudioTemplates\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A5B2BE-E1E4-4FCB-92C5-52FB64865928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2302EF1-D7A2-4181-8402-9532C3AD39A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -656,9 +656,6 @@
     <t>Storage Bucket Name (required when Action Center is used). Has a corresponding asset that can be configured to overwrite this setting.</t>
   </si>
   <si>
-    <t>Path inside  the Storage Bucket where actions will store the files. Has a corresponding asset that can be configured to overwrite this setting.</t>
-  </si>
-  <si>
     <t>The name of the Orchestrator Queue. Has a corresponding asset that can be configured to overwrite this setting.</t>
   </si>
   <si>
@@ -791,58 +788,61 @@
     <t>OCR Autocorrection finished</t>
   </si>
   <si>
+    <t>AutocorrectStorageBucketDirectoryPath</t>
+  </si>
+  <si>
+    <t>Path inside the Storage Bucket where actions will store the files. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>Path inside the Storage Bucket where the autocorrect file is stored. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>DU_AutocorrectStorageBucketDirectoryPath</t>
+  </si>
+  <si>
     <t>Path inside the Storage Bucket where actions will store the files. The asset value overrides the one from the "Settings" sheet</t>
   </si>
   <si>
-    <t>AutocorrectStorageBucketDirectoryPath</t>
-  </si>
-  <si>
-    <t>DU_AutocorrectStorageBucketDirectoryPath</t>
+    <t>MinimumNumberOfRepetitions</t>
+  </si>
+  <si>
+    <t>AutocorrectionEnabled</t>
+  </si>
+  <si>
+    <t>A flag that determines if autocorrection should be called or not. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>The minimum number of times the value needs to be corrected in Action Center before the flow will start to autocorrect. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>DU_MinimumNumberOfRepetitions</t>
+  </si>
+  <si>
+    <t>DU_AutocorrectionEnabled</t>
   </si>
   <si>
     <t>Path inside the Storage Bucket where the autocorrect file is stored. The asset value overrides the one from the "AutocorrectOcrMistakes" sheet</t>
   </si>
   <si>
-    <t>MinimumNumberOfRepetitions</t>
-  </si>
-  <si>
-    <t>DU_MinimumNumberOfRepetitions</t>
-  </si>
-  <si>
     <t>The minimum number of times the value needs to be corrected in Action Center before the flow will start to autocorrect. The asset value overrides the one from the "AutocorrectOcrMistakes" sheet</t>
   </si>
   <si>
-    <t>AutocorrectionEnabled</t>
-  </si>
-  <si>
-    <t>DU_AutocorrectionEnabled</t>
+    <t>AutocorrectionFieldName</t>
+  </si>
+  <si>
+    <t>The name of the field we want to enable autocorrection for. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>DU_AutocorrectionFieldName</t>
   </si>
   <si>
     <t>A flag that determines if autocorrection should be called or not. The asset value overrides the one from the "AutocorrectOcrMistakes" sheet</t>
   </si>
   <si>
-    <t>AutocorrectionFieldName</t>
-  </si>
-  <si>
-    <t>DU_AutocorrectionFieldName</t>
-  </si>
-  <si>
     <t>The name of the field we want to enable autocorrection for. The asset value overrides the one from the "AutocorrectOcrMistakes" sheet</t>
   </si>
   <si>
     <t>AutocorrectionLearningFile</t>
-  </si>
-  <si>
-    <t>Path inside the Storage Bucket where the autocorrect file is stored. Has a corresponding asset that can be configured to overwrite this setting.</t>
-  </si>
-  <si>
-    <t>The minimum number of times the value needs to be corrected in Action Center before the flow will start to autocorrect. Has a corresponding asset that can be configured to overwrite this setting.</t>
-  </si>
-  <si>
-    <t>A flag that determines if autocorrection should be called or not. Has a corresponding asset that can be configured to overwrite this setting.</t>
-  </si>
-  <si>
-    <t>The name of the field we want to enable autocorrection for. Has a corresponding asset that can be configured to overwrite this setting.</t>
   </si>
 </sst>
 </file>
@@ -1242,16 +1242,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="43.90625" customWidth="1"/>
     <col min="2" max="2" width="70.08984375" customWidth="1"/>
-    <col min="3" max="3" width="131.7265625" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="131.81640625" customWidth="1"/>
+    <col min="4" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1419,13 +1419,13 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B14" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C14" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1481,13 +1481,13 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B22">
         <v>0.5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1495,13 +1495,13 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>237</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" t="s">
         <v>239</v>
-      </c>
-      <c r="C24" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1538,7 +1538,7 @@
         <v>114</v>
       </c>
       <c r="C29" t="s">
-        <v>206</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1546,10 +1546,10 @@
         <v>78</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1557,7 +1557,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2542,10 +2542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1019"/>
+  <dimension ref="A1:Z1021"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2553,7 +2553,7 @@
     <col min="1" max="1" width="56" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="116.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="4" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2845,18 +2845,18 @@
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>246</v>
+      </c>
+      <c r="B34" t="s">
         <v>247</v>
-      </c>
-      <c r="B34" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>248</v>
+      </c>
+      <c r="B35" t="s">
         <v>249</v>
-      </c>
-      <c r="B35" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2944,18 +2944,18 @@
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
+        <v>233</v>
+      </c>
+      <c r="B49" t="s">
         <v>234</v>
-      </c>
-      <c r="B49" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
+        <v>235</v>
+      </c>
+      <c r="B50" t="s">
         <v>236</v>
-      </c>
-      <c r="B50" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2984,10 +2984,10 @@
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
+        <v>240</v>
+      </c>
+      <c r="B54" t="s">
         <v>241</v>
-      </c>
-      <c r="B54" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3999,6 +3999,8 @@
     <row r="1017" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1018" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1019" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1020" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1021" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4008,10 +4010,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA1001"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4160,7 +4162,7 @@
         <v>193</v>
       </c>
       <c r="D11" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4187,25 +4189,25 @@
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>253</v>
       </c>
       <c r="D16" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4213,32 +4215,32 @@
         <v>255</v>
       </c>
       <c r="B17" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="D17" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B18" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D18" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B19" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D19" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5222,7 +5224,6 @@
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5230,21 +5231,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3556146-5150-42C6-A923-4DA70213A01F}">
-  <dimension ref="A1:C29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D9E9D1-D414-4B7E-8E38-DC0DB03EC0B3}">
+  <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="43.90625" customWidth="1"/>
     <col min="2" max="2" width="70.08984375" customWidth="1"/>
     <col min="3" max="3" width="166" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5254,24 +5256,71 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C3" t="s">
         <v>252</v>
       </c>
-      <c r="B3" t="s">
-        <v>264</v>
-      </c>
-      <c r="C3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>255</v>
       </c>
@@ -5279,74 +5328,1059 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C7" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="5"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="5"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="5"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="5"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="5"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="2"/>
     </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="68" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="69" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="70" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="71" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="72" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="73" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="74" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="75" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="76" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="77" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="78" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="79" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="100" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="101" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="102" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="103" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="104" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="105" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="106" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="107" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="108" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="109" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="110" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="111" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="112" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="113" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="114" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="115" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="116" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="117" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="118" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="119" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="120" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="121" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="122" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="123" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="124" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="125" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="126" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="127" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="128" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="129" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="130" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="131" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="132" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="133" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="134" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="135" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="136" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="137" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="138" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="139" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="140" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="141" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="142" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="143" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="144" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="145" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="146" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="147" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="148" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="149" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="150" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="151" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="152" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="153" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="154" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="155" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="156" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="157" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="158" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="159" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="160" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="161" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="162" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="163" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="164" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="165" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="166" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="167" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="168" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="169" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="170" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="171" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="172" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="173" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="174" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="175" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="176" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="177" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="178" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="179" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="180" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="181" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="182" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="183" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="184" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="185" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="186" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="187" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="188" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="189" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="190" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="191" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="192" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="193" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="194" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="195" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="196" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="197" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="198" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="199" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="200" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="201" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="202" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="203" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="204" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="205" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="206" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="207" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="208" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5563,15 +6597,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D1FA23-0F05-4B8D-B77D-DF9AB2091E72}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="60.26953125" customWidth="1"/>
+    <col min="1" max="1" width="60.1796875" customWidth="1"/>
     <col min="2" max="2" width="79.36328125" customWidth="1"/>
-    <col min="3" max="3" width="221.26953125" customWidth="1"/>
+    <col min="3" max="3" width="221.1796875" customWidth="1"/>
     <col min="4" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5588,15 +6622,15 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
         <v>212</v>
-      </c>
-      <c r="B3" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" t="s">
         <v>126</v>
@@ -5604,7 +6638,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B5" t="s">
         <v>128</v>
@@ -5612,7 +6646,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" t="s">
         <v>134</v>
@@ -5620,7 +6654,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -5628,15 +6662,15 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" t="s">
         <v>218</v>
-      </c>
-      <c r="B8" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B10" t="s">
         <v>142</v>
@@ -5644,10 +6678,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" t="s">
         <v>221</v>
-      </c>
-      <c r="B12" t="s">
-        <v>222</v>
       </c>
       <c r="C12" t="s">
         <v>144</v>
@@ -5655,10 +6689,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" t="s">
         <v>223</v>
-      </c>
-      <c r="B13" t="s">
-        <v>224</v>
       </c>
       <c r="C13" t="s">
         <v>146</v>
@@ -5666,10 +6700,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>224</v>
+      </c>
+      <c r="B14" t="s">
         <v>225</v>
-      </c>
-      <c r="B14" t="s">
-        <v>226</v>
       </c>
       <c r="C14" t="s">
         <v>148</v>
@@ -5677,10 +6711,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" t="s">
         <v>227</v>
-      </c>
-      <c r="B15" t="s">
-        <v>228</v>
       </c>
       <c r="C15" t="s">
         <v>150</v>
@@ -5688,10 +6722,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" t="s">
         <v>229</v>
-      </c>
-      <c r="B16" t="s">
-        <v>230</v>
       </c>
       <c r="C16" t="s">
         <v>152</v>
@@ -5699,7 +6733,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B18">
         <v>50</v>
@@ -5707,7 +6741,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B19">
         <v>85</v>
@@ -5715,7 +6749,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B20">
         <v>50</v>

</xml_diff>

<commit_message>
Update Config_Expected.xlsx file, removed Currency.
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/Config_Expected.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/Config_Expected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\add_pytest_v2\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Tests\Cache\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\Develop\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Tests\Cache\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D2637F-3EDB-418C-AAAD-BDA5E813EDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5909AC27-75BB-41D9-B027-5B3DECEDB349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12828" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -524,9 +524,6 @@
     <t>PO Number-Confidence</t>
   </si>
   <si>
-    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms, Currency,Discount</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
@@ -852,6 +849,9 @@
   </si>
   <si>
     <t>RetryIntervalLow</t>
+  </si>
+  <si>
+    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms,Discount</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1333,7 @@
         <v>110</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1428,59 +1428,59 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>179</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1490,13 +1490,13 @@
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B22">
         <v>0.5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1504,13 +1504,13 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>238</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" t="s">
         <v>240</v>
-      </c>
-      <c r="C24" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1522,7 +1522,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1530,7 +1530,7 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1547,7 +1547,7 @@
         <v>114</v>
       </c>
       <c r="C29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1555,10 +1555,10 @@
         <v>78</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1566,7 +1566,7 @@
         <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2553,7 +2553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -2646,13 +2646,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B7">
         <v>99999</v>
       </c>
       <c r="C7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2679,7 +2679,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2751,7 +2751,7 @@
         <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2767,7 +2767,7 @@
         <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2775,7 +2775,7 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2791,7 +2791,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2831,7 +2831,7 @@
         <v>77</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2847,7 +2847,7 @@
         <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2863,7 +2863,7 @@
         <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2876,18 +2876,18 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>264</v>
+      </c>
+      <c r="B36" t="s">
         <v>265</v>
-      </c>
-      <c r="B36" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>266</v>
+      </c>
+      <c r="B37" t="s">
         <v>267</v>
-      </c>
-      <c r="B37" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2908,18 +2908,18 @@
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2975,18 +2975,18 @@
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>234</v>
+      </c>
+      <c r="B51" t="s">
         <v>235</v>
-      </c>
-      <c r="B51" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>236</v>
+      </c>
+      <c r="B52" t="s">
         <v>237</v>
-      </c>
-      <c r="B52" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3015,10 +3015,10 @@
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>241</v>
+      </c>
+      <c r="B56" t="s">
         <v>242</v>
-      </c>
-      <c r="B56" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3035,7 +3035,7 @@
         <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3044,7 +3044,7 @@
         <v>55</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3069,7 +3069,7 @@
         <v>31</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4105,46 +4105,46 @@
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4157,10 +4157,10 @@
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4168,10 +4168,10 @@
         <v>36</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4179,10 +4179,10 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4190,10 +4190,10 @@
         <v>114</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4201,10 +4201,10 @@
         <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4212,66 +4212,66 @@
         <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D16" t="s">
         <v>257</v>
-      </c>
-      <c r="D16" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B17" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" t="s">
         <v>259</v>
-      </c>
-      <c r="D17" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B18" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" t="s">
         <v>261</v>
-      </c>
-      <c r="D18" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D19" t="s">
         <v>263</v>
-      </c>
-      <c r="D19" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5266,8 +5266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5417,7 +5417,7 @@
         <v>151</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>162</v>
+        <v>271</v>
       </c>
       <c r="C19" t="s">
         <v>152</v>
@@ -5498,15 +5498,15 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" t="s">
         <v>213</v>
-      </c>
-      <c r="B3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B4" t="s">
         <v>126</v>
@@ -5514,7 +5514,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B5" t="s">
         <v>128</v>
@@ -5522,7 +5522,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B6" t="s">
         <v>134</v>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
         <v>138</v>
@@ -5538,15 +5538,15 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
         <v>219</v>
-      </c>
-      <c r="B8" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s">
         <v>142</v>
@@ -5554,10 +5554,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" t="s">
         <v>222</v>
-      </c>
-      <c r="B12" t="s">
-        <v>223</v>
       </c>
       <c r="C12" t="s">
         <v>144</v>
@@ -5565,10 +5565,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" t="s">
         <v>224</v>
-      </c>
-      <c r="B13" t="s">
-        <v>225</v>
       </c>
       <c r="C13" t="s">
         <v>146</v>
@@ -5576,10 +5576,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>225</v>
+      </c>
+      <c r="B14" t="s">
         <v>226</v>
-      </c>
-      <c r="B14" t="s">
-        <v>227</v>
       </c>
       <c r="C14" t="s">
         <v>148</v>
@@ -5587,10 +5587,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B15" t="s">
         <v>228</v>
-      </c>
-      <c r="B15" t="s">
-        <v>229</v>
       </c>
       <c r="C15" t="s">
         <v>150</v>
@@ -5598,10 +5598,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" t="s">
         <v>230</v>
-      </c>
-      <c r="B16" t="s">
-        <v>231</v>
       </c>
       <c r="C16" t="s">
         <v>152</v>
@@ -5609,7 +5609,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B18">
         <v>50</v>
@@ -5617,7 +5617,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B19">
         <v>85</v>
@@ -5625,7 +5625,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B20">
         <v>50</v>
@@ -5716,44 +5716,44 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" t="s">
         <v>248</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>249</v>
-      </c>
-      <c r="C3" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B5">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" t="s">
         <v>255</v>
-      </c>
-      <c r="C7" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Windows VB - Add variable description for AutocorrectOcrMistakes.xaml; add missing asset in config; update Config_Expected.xlsx; Add AutocorrectionLearningFile.json; update Python tests data; Cross-platform - Add AutocorrectionLearningFile.json; add missing asset in config;
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/Config_Expected.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/Config_Expected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\Develop\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Tests\Cache\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\Cross_platform\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5909AC27-75BB-41D9-B027-5B3DECEDB349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C369CC-C0D2-4ACF-9956-E974F6E6C10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9468" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="271">
   <si>
     <t>Name</t>
   </si>
@@ -782,9 +782,6 @@
     <t>AutocorrectStorageBucketDirectoryPath</t>
   </si>
   <si>
-    <t>AutocorrectionLearningFile</t>
-  </si>
-  <si>
     <t>Path inside the Storage Bucket where the autocorrect file is stored. Has a corresponding asset that can be configured to overwrite this setting.</t>
   </si>
   <si>
@@ -800,12 +797,6 @@
     <t>A flag that determines if autocorrection should be called or not. Has a corresponding asset that can be configured to overwrite this setting.</t>
   </si>
   <si>
-    <t>AutocorrectionFieldName</t>
-  </si>
-  <si>
-    <t>The name of the field we want to enable autocorrection for. Has a corresponding asset that can be configured to overwrite this setting.</t>
-  </si>
-  <si>
     <t>DU_AutocorrectStorageBucketDirectoryPath</t>
   </si>
   <si>
@@ -824,12 +815,6 @@
     <t>A flag that determines if autocorrection should be called or not. The asset value overrides the one from the "AutocorrectOcrMistakes" sheet</t>
   </si>
   <si>
-    <t>DU_AutocorrectionFieldName</t>
-  </si>
-  <si>
-    <t>The name of the field we want to enable autocorrection for. The asset value overrides the one from the "AutocorrectOcrMistakes" sheet</t>
-  </si>
-  <si>
     <t>LogMessage_AutocorrectOcrMistakesStart</t>
   </si>
   <si>
@@ -852,6 +837,18 @@
   </si>
   <si>
     <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms,Discount</t>
+  </si>
+  <si>
+    <t>AutocorrectionLearningFile.json</t>
+  </si>
+  <si>
+    <t>AutocorrectionFieldIdList</t>
+  </si>
+  <si>
+    <t>A comma separated list of the taxonomy ids of the fields we want to enable autocorrection for. Has a corresponding asset that can be configured to overwrite this setting.</t>
+  </si>
+  <si>
+    <t>DU_AutocorrectionFieldIdList</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1249,7 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2553,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1023"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2646,13 +2643,13 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B7">
         <v>99999</v>
       </c>
       <c r="C7" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2679,7 +2676,7 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -2876,18 +2873,18 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B36" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B37" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4043,8 +4040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4235,43 +4232,43 @@
         <v>247</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B17" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D17" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B18" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D18" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="B19" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="D19" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5266,8 +5263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5007CE1-A05D-4745-B7EA-4E0BD0A3B111}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5417,7 +5414,7 @@
         <v>151</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="C19" t="s">
         <v>152</v>
@@ -5474,7 +5471,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5640,8 +5637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{419DF484-C338-43D9-B349-5A8AB18C6D9F}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5719,41 +5716,41 @@
         <v>247</v>
       </c>
       <c r="B3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" t="s">
         <v>248</v>
-      </c>
-      <c r="C3" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>250</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="C7" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Windows VB - Python test correction
</commit_message>
<xml_diff>
--- a/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/Config_Expected.xlsx
+++ b/DocumentUnderstandingProcess/contentFiles/any/any/pt0/VisualBasic/Tests/Cache/Config_Expected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\teodora.patrascu\PycharmProjects\Cross_platform\DocumentUnderstandingProcess\contentFiles\any\any\pt0\VisualBasic\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C369CC-C0D2-4ACF-9956-E974F6E6C10A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0DF345-8765-405C-AFF6-B1BB63538D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9468" yWindow="-17388" windowWidth="30936" windowHeight="17040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21252" yWindow="-17568" windowWidth="30936" windowHeight="17040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="274">
   <si>
     <t>Name</t>
   </si>
@@ -836,9 +836,6 @@
     <t>RetryIntervalLow</t>
   </si>
   <si>
-    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms,Discount</t>
-  </si>
-  <si>
     <t>AutocorrectionLearningFile.json</t>
   </si>
   <si>
@@ -849,6 +846,18 @@
   </si>
   <si>
     <t>DU_AutocorrectionFieldIdList</t>
+  </si>
+  <si>
+    <t>DU_DateFormats</t>
+  </si>
+  <si>
+    <t>Different date formats.</t>
+  </si>
+  <si>
+    <t>yyyy-MM-dd;dd-MM-yyyy;MM-dd-yyyy;MM/dd/yyyy;dd/MM/yyyy;yyyy/MM/dd;dd.MM.yyyy;MM.dd.yyyy;yyyy.MM.dd</t>
+  </si>
+  <si>
+    <t>Tax Amount,Net Amount,Discount,Shipping Charges,Billing Name,Total, Name, Vendor Address, Billing Address, Billing VAT Number, Payment Address, Vendor VAT Number, DueDate,Payment Terms</t>
   </si>
 </sst>
 </file>
@@ -1246,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="B5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1435,138 +1444,150 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>162</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>178</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>184</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="2"/>
+      <c r="A21" t="s">
+        <v>209</v>
+      </c>
+      <c r="B21">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>209</v>
-      </c>
-      <c r="B22">
-        <v>0.5</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>210</v>
-      </c>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="2"/>
+      <c r="A23" t="s">
+        <v>238</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>238</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C24" t="s">
-        <v>240</v>
-      </c>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
+      <c r="A25" t="s">
+        <v>270</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C25" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>35</v>
-      </c>
       <c r="B26" s="2"/>
-      <c r="C26" t="s">
-        <v>203</v>
-      </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B27" s="2"/>
       <c r="C27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="2"/>
+        <v>36</v>
+      </c>
       <c r="C28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>114</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B29" s="2"/>
       <c r="C29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>245</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>79</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2540,6 +2561,7 @@
     <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4041,7 +4063,7 @@
   <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4262,17 +4284,27 @@
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19" t="s">
+        <v>269</v>
+      </c>
+      <c r="D19" t="s">
         <v>268</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>270</v>
       </c>
-      <c r="D19" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B21" t="s">
+        <v>270</v>
+      </c>
+      <c r="D21" t="s">
+        <v>271</v>
+      </c>
+    </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5264,7 +5296,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5414,7 +5446,7 @@
         <v>151</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="C19" t="s">
         <v>152</v>
@@ -5716,7 +5748,7 @@
         <v>247</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C3" t="s">
         <v>248</v>
@@ -5747,10 +5779,10 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C7" t="s">
         <v>268</v>
-      </c>
-      <c r="C7" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>